<commit_message>
Update project documentation and improve data exporting capabilities
Updates project documentation PDF and adds the ability to export comments to Excel.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ac4cc178-77a1-4ab9-bb41-2e7b8c963745
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3c05d6ac-6c78-4b71-b159-2c1ba84aed9a/b55f8aae-f0b1-4756-9aac-b9ffdfdc8019.jpg
</commit_message>
<xml_diff>
--- a/excel_exports/visitors.xlsx
+++ b/excel_exports/visitors.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1330,6 +1330,1106 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>admin_dashboard</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:16:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) HeadlessChrome/118.0.5993.88 ...</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) HeadlessChrome/118.0.5993.88 ...</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) HeadlessChrome/118.0.5993.88 ...</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) HeadlessChrome/118.0.5993.88 ...</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>vote_comment</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>vote_comment</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>vote_comment</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>admin_dashboard</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:18:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>delete_topic</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>admin_dashboard</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>admin_dashboard</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>31.94.64.109</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 18_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Mobi...</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>delete_topic</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2025-07-03 16:19:12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>